<commit_message>
mod xlsx add xlsx
OK!
</commit_message>
<xml_diff>
--- a/folder2/test/test.xlsx
+++ b/folder2/test/test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="30" windowWidth="19200" windowHeight="12090"/>
@@ -11,8 +11,17 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>tets2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -354,12 +363,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:2">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>